<commit_message>
chore: add new sheet 3
</commit_message>
<xml_diff>
--- a/one-sheet-multiple-table.xlsx
+++ b/one-sheet-multiple-table.xlsx
@@ -5,6 +5,7 @@
   <sheets>
     <sheet state="visible" name="Sheet1" sheetId="1" r:id="rId4"/>
     <sheet state="visible" name="Sheet2" sheetId="2" r:id="rId5"/>
+    <sheet state="visible" name="Sheet3" sheetId="3" r:id="rId6"/>
   </sheets>
   <definedNames/>
   <calcPr/>
@@ -12,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="24">
   <si>
     <t>no</t>
   </si>
@@ -75,6 +76,15 @@
   </si>
   <si>
     <t>Laptop</t>
+  </si>
+  <si>
+    <t>Klare</t>
+  </si>
+  <si>
+    <t>Hary</t>
+  </si>
+  <si>
+    <t>Ozil</t>
   </si>
 </sst>
 </file>
@@ -128,6 +138,10 @@
 </file>
 
 <file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
 </file>
 
@@ -529,4 +543,189 @@
   </sheetData>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="0" summaryRight="0"/>
+  </sheetPr>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="C2" s="1">
+        <v>2020.0</v>
+      </c>
+      <c r="D2" s="1">
+        <v>2021.0</v>
+      </c>
+      <c r="E2" s="1">
+        <v>2022.0</v>
+      </c>
+      <c r="F2" s="1">
+        <v>2023.0</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="1">
+        <v>1.0</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C3" s="1">
+        <v>23.0</v>
+      </c>
+      <c r="D3" s="1">
+        <v>24.0</v>
+      </c>
+      <c r="E3" s="1">
+        <v>25.0</v>
+      </c>
+      <c r="F3" s="1">
+        <v>26.0</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="1">
+        <v>2.0</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C4" s="1">
+        <v>24.0</v>
+      </c>
+      <c r="D4" s="1">
+        <v>25.0</v>
+      </c>
+      <c r="E4" s="1">
+        <v>26.0</v>
+      </c>
+      <c r="F4" s="1">
+        <v>27.0</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="1">
+        <v>3.0</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C5" s="1">
+        <v>24.0</v>
+      </c>
+      <c r="D5" s="1">
+        <v>25.0</v>
+      </c>
+      <c r="E5" s="1">
+        <v>26.0</v>
+      </c>
+      <c r="F5" s="1">
+        <v>27.0</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="1">
+        <v>4.0</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C6" s="1">
+        <v>43.0</v>
+      </c>
+      <c r="D6" s="1">
+        <v>44.0</v>
+      </c>
+      <c r="E6" s="1">
+        <v>45.0</v>
+      </c>
+      <c r="F6" s="1">
+        <v>46.0</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="1">
+        <v>5.0</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C7" s="1">
+        <v>54.0</v>
+      </c>
+      <c r="D7" s="1">
+        <v>55.0</v>
+      </c>
+      <c r="E7" s="1">
+        <v>56.0</v>
+      </c>
+      <c r="F7" s="1">
+        <v>57.0</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="1">
+        <v>6.0</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C8" s="1">
+        <v>32.0</v>
+      </c>
+      <c r="D8" s="1">
+        <v>33.0</v>
+      </c>
+      <c r="E8" s="1">
+        <v>34.0</v>
+      </c>
+      <c r="F8" s="1">
+        <v>35.0</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="1">
+        <v>7.0</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C9" s="1">
+        <v>12.0</v>
+      </c>
+      <c r="D9" s="1">
+        <v>13.0</v>
+      </c>
+      <c r="E9" s="1">
+        <v>14.0</v>
+      </c>
+      <c r="F9" s="1">
+        <v>15.0</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="C1:F1"/>
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="B1:B2"/>
+  </mergeCells>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>